<commit_message>
feat: Update AI features, task details, and tests
</commit_message>
<xml_diff>
--- a/tests/e2e/downloads/cjk_en-US.xlsx
+++ b/tests/e2e/downloads/cjk_en-US.xlsx
@@ -1,55 +1,99 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="任务列表" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Tasks" state="visible" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+  <si>
+    <t>Hierarchy</t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Duration (days)</t>
+  </si>
+  <si>
+    <t>Progress (%)</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>actual_start</t>
+  </si>
+  <si>
+    <t>actual_end</t>
+  </si>
+  <si>
+    <t>actual_hours</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>项目α-プロジェクト-프로젝트-Project</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2023-06-01</t>
+  </si>
+  <si>
+    <t>2023-06-08</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0E0E0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,14 +108,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,66 +449,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M100"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="8" width="10" customWidth="1"/>
+    <col min="9" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Hierarchy</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Task Name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Priority</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Assignee</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Start Date</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Duration (days)</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Progress (%)</v>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <v>项目α-プロジェクト-프로젝트-Project</v>
-      </c>
-      <c r="C2" t="str">
-        <v/>
-      </c>
-      <c r="D2" t="str">
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <v/>
-      </c>
-      <c r="F2" t="str">
-        <v>2023-06-01</v>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -463,10 +527,150 @@
       <c r="H2">
         <v>0</v>
       </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
     </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="3:8" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="3:8" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
-  </ignoredErrors>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="warning" errorTitle="Invalid Input" error="Please select from the list" sqref="C10:C100">
+      <formula1>"High,Medium,Low"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="warning" errorTitle="Invalid Input" error="Please select from the list" sqref="C2:C100">
+      <formula1>"High,Medium,Low"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="warning" errorTitle="Invalid Input" error="Please select from the list" sqref="E10:E100">
+      <formula1>"Pending,In Progress,Completed,Cancelled"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="warning" errorTitle="Invalid Input" error="Please select from the list" sqref="E2:E100">
+      <formula1>"Pending,In Progress,Completed,Cancelled"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Input" error="Please enter a valid number" sqref="G10:G100">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Input" error="Please enter a valid number" sqref="G2:G100">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Input" error="Progress must be between 0 and 100" sqref="H10:H100">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Invalid Input" error="Progress must be between 0 and 100" sqref="H2:H100">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>